<commit_message>
gjort om funktionalitet för att lääga till en medlem
</commit_message>
<xml_diff>
--- a/SprintBacklog.xlsx
+++ b/SprintBacklog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>1. Ta bort medlem</t>
+  </si>
+  <si>
+    <t>6. Implementering av inläsnig av textfil för sparning av medlemmar.</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +512,9 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -523,6 +529,9 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
+      <c r="E3" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -537,6 +546,9 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
+      <c r="E4" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -551,6 +563,9 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -560,10 +575,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -588,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -637,106 +655,128 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
+      <c r="A12" s="1">
+        <v>6</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>7.5</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixat den mesta funktionaliteten
</commit_message>
<xml_diff>
--- a/SprintBacklog.xlsx
+++ b/SprintBacklog.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -597,6 +597,9 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -611,6 +614,9 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -625,6 +631,9 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -639,6 +648,9 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -653,6 +665,9 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -668,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>